<commit_message>
Add more functions to GUI
</commit_message>
<xml_diff>
--- a/configs-matlab1.xlsx
+++ b/configs-matlab1.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sshafaamri\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -98,12 +93,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -193,7 +188,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -228,7 +223,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -443,9 +438,9 @@
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -474,7 +469,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -515,7 +510,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -559,7 +554,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -603,7 +598,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -647,7 +642,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -691,7 +686,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -735,7 +730,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
         <v>19</v>
       </c>
@@ -767,7 +762,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>5</v>
       </c>
@@ -805,13 +800,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -840,7 +835,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -881,7 +876,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -925,7 +920,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -954,7 +949,7 @@
         <v>0.65418467223967969</v>
       </c>
       <c r="J4">
-        <v>0.55991546779480572</v>
+        <v>0.59470028437458211</v>
       </c>
       <c r="K4">
         <v>0.72063650542960955</v>
@@ -969,7 +964,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1013,7 +1008,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1057,7 +1052,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1077,7 +1072,7 @@
         <v>0.74866602803860749</v>
       </c>
       <c r="G7">
-        <v>0.55991546779480572</v>
+        <v>0.59470028437458211</v>
       </c>
       <c r="H7">
         <v>0.92898486361039223</v>
@@ -1101,7 +1096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
         <v>19</v>
       </c>
@@ -1133,7 +1128,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>5</v>
       </c>
@@ -1171,13 +1166,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1206,7 +1201,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1247,7 +1242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1291,7 +1286,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1335,7 +1330,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1379,7 +1374,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1423,7 +1418,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1467,7 +1462,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
         <v>19</v>
       </c>
@@ -1499,7 +1494,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>5</v>
       </c>

</xml_diff>